<commit_message>
late, but correct final leaderboard
</commit_message>
<xml_diff>
--- a/Spring Challenge 2024 Standings.xlsx
+++ b/Spring Challenge 2024 Standings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwj/Documents/MAPS/Oppgaver-Spring-Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A0DAE6-9E4B-7543-BA90-2D36F2D38D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE5FB29-8ECB-1C48-BE3C-68246EBFA4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C7474919-35BA-42A8-AC49-73C7A03ECD77}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{C7474919-35BA-42A8-AC49-73C7A03ECD77}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>CYB Bursdag</t>
   </si>
@@ -104,13 +104,37 @@
   </si>
   <si>
     <t>MAMI2</t>
+  </si>
+  <si>
+    <t>3(2)</t>
+  </si>
+  <si>
+    <t>3(1)</t>
+  </si>
+  <si>
+    <t>1(1)3</t>
+  </si>
+  <si>
+    <t>1(2)3</t>
+  </si>
+  <si>
+    <t>AMAVIM</t>
+  </si>
+  <si>
+    <t>Narvesen veganchorizo</t>
+  </si>
+  <si>
+    <t>4(2)</t>
+  </si>
+  <si>
+    <t>4(1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +145,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,6 +293,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,6 +309,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -594,7 +631,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,42 +682,46 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="8"/>
@@ -688,29 +729,47 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -720,12 +779,14 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -733,71 +794,75 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="I7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>

</xml_diff>